<commit_message>
update the excel sheet
</commit_message>
<xml_diff>
--- a/tools/cmmc/cmmc-v2.xlsx
+++ b/tools/cmmc/cmmc-v2.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F3A570-34E4-3F4B-98E6-E8B1D39E856A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D99FFB-6934-8741-98B2-ED7E7CAE2CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20340" tabRatio="792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3860" yWindow="-28300" windowWidth="51200" windowHeight="28300" tabRatio="792" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="103" r:id="rId1"/>
     <sheet name="cmmc" sheetId="102" r:id="rId2"/>
+    <sheet name="levels" sheetId="104" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="510">
   <si>
     <t>AC</t>
   </si>
@@ -693,9 +694,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>maturity</t>
-  </si>
-  <si>
     <t>AC.L1-3.1.1</t>
   </si>
   <si>
@@ -1366,13 +1364,684 @@
   </si>
   <si>
     <t>urn:intuitem:risk:framework:cmmc-2.0</t>
+  </si>
+  <si>
+    <t>annotation</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] authorized users are identified;
+[b] processes acting on behalf of authorized users are identified;
+[c] devices (and other systems) authorized to connect to the system are identified;
+[d] system access is limited to authorized users;
+[e] system access is limited to processes acting on behalf of authorized users; and
+[f] system access is limited to authorized devices (including other systems).</t>
+  </si>
+  <si>
+    <t>implementation_groups</t>
+  </si>
+  <si>
+    <t>levels</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the types of transactions and functions that authorized users are permitted to execute are defined; and
+[b] system access is limited to the defined types of transactions and functions for authorized users.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] connections to external systems are identified;
+[b] the use of external systems is identified;
+[c] connections to external systems are verified;
+[d] the use of external systems is verified;
+[e] connections to external systems are controlled/limited; and
+[f] the use of external systems is controlled/limited.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] individuals authorized to post or process information on publicly accessible systems are identified;
+[b] procedures to ensure FCI is not posted or processed on publicly accessible systems are identified;
+[c] a review process is in place prior to posting of any content to publicly accessible systems;
+[d] content on publicly accessible systems is reviewed to ensure that it does not include FCI; and
+[e] mechanisms are in place to remove and address improper posting of FCI.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] system users are identified;
+[b] processes acting on behalf of users are identified; and
+[c] devices accessing the system are identified.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the identity of each user is authenticated or verified as a prerequisite to system access;
+[b] the identity of each process acting on behalf of a user is authenticated or verified as a prerequisite to system access; and
+[c] the identity of each device accessing or connecting to the system is authenticated or verified as a prerequisite to system access.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a]system media containing FCI is sanitized or destroyed before disposal; and
+[b]system media containing FCI is sanitized before it is released for reuse.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] authorized individuals allowed physical access are identified;
+[b] physical access to organizational systems is limited to authorized individuals;
+[c] physical access to equipment is limited to authorized individuals; and
+[d] physical access to operating environments is limited to authorized individuals.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] visitors are escorted; and
+[b] visitor activity is monitored.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] audit logs of physical access are maintained.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] physical access devices are identified;
+[b] physical access devices are controlled; and
+[c] physical access devices are managed.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the external system boundary is defined;
+[b] key internal system boundaries are defined;
+[c] communications are monitored at the external system boundary;
+[d] communications are monitored at key internal boundaries;
+[e] communications are controlled at the external system boundary;
+[f] communications are controlled at key internal boundaries;
+[g] communications are protected at the external system boundary; and
+[h] communications are protected at key internal boundaries.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] publicly accessible system components are identified; and
+[b] subnetworks for publicly accessible system components are physically or logically separated from internal networks.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the time within which to identify system flaws is specified;
+[b] system flaws are identified within the specified time frame;
+[c] the time within which to report system flaws is specified;
+[d] system flaws are reported within the specified time frame;
+[e] the time within which to correct system flaws is specified; and
+[f] system flaws are corrected within the specified time frame.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] designated locations for malicious code protection are identified; and
+[b] protection from malicious code at designated locations is provided.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] malicious code protection mechanisms are updated when new releases are available.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the frequency for malicious code scans is defined;
+[b] malicious code scans are performed with the defined frequency; and
+[c] real-time malicious code scans of files from external sources as files are downloaded, opened, or executed are performed.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] information flow control policies are defined;
+[b] methods and enforcement mechanisms for controlling the flow of CUI are defined;
+[c] designated sources and destinations (e.g., networks, individuals, and devices) for CUI within the system and between interconnected systems are identified;
+[d] authorizations for controlling the flow of CUI are defined; and
+[e] approved authorizations for controlling the flow of CUI are enforced.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the duties of individuals requiring separation are defined;
+[b] responsibilities for duties that require separation are assigned to separate individuals; and
+[c] access privileges that enable individuals to exercise the duties that require separation are granted to separate individuals.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] privileged accounts are identified;
+[b] access to privileged accounts is authorized in accordance with the principle of least privilege;
+[c] security functions are identified; and
+[d] access to security functions is authorized in accordance with the principle of least privilege.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] nonsecurity functions are identified; and
+[b] users are required to use non-privileged accounts or roles when accessing nonsecurity functions.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] privileged functions are defined;
+[b] non-privileged users are defined;
+[c] non-privileged users are prevented from executing privileged functions; and
+[d] the execution of privileged functions is captured in audit logs.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the means of limiting unsuccessful logon attempts is defined; and
+[b] the defined means of limiting unsuccessful logon attempts is implemented.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] privacy and security notices required by CUI-specified rules are identified, consistent, and associated with the specific CUI category; and
+[b] privacy and security notices are displayed.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the period of inactivity after which the system initiates a session lock is defined;
+[b] access to the system and viewing of data is prevented by initiating a session lock after the defined period of inactivity; and
+[c] previously visible information is concealed via a pattern-hiding display after the defined period of inactivity.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] conditions requiring a user session to terminate are defined; and
+[b] a user session is automatically terminated after any of the defined conditions occur.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] remote access sessions are permitted;
+[b] the types of permitted remote access are identified;
+[c] remote access sessions are controlled; and
+[d] remote access sessions are monitored.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] cryptographic mechanisms to protect the confidentiality of remote access sessions are identified; and
+[b] cryptographic mechanisms to protect the confidentiality of remote access sessions are implemented.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] managed access control points are identified and implemented; and
+[b] remote access is routed through managed network access control points.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] privileged commands authorized for remote execution are identified;
+[b] security-relevant information authorized to be accessed remotely is identified;
+[c] the execution of the identified privileged commands via remote access is authorized; and
+[d] access to the identified security-relevant information via remote access is authorized.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] wireless access points are identified; and
+[b] wireless access is authorized prior to allowing such connections.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] wireless access to the system is protected using authentication; and
+[b] wireless access to the system is protected using encryption.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] mobile devices that process, store, or transmit CUI are identified;
+[b] mobile device connections are authorized; and
+[c] mobile device connections are monitored and logged.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] mobile devices and mobile computing platforms that process, store, or transmit CUI are identified; and
+[b] encryption is employed to protect CUI on identified mobile devices and mobile computing platforms.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the use of portable storage devices containing CUI on external systems is identified and documented;
+[b] limits on the use of portable storage devices containing CUI on external systems are defined; and
+[c] the use of portable storage devices containing CUI on external systems is limited as defined.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] security risks associated with organizational activities involving CUI are identified;
+[b] policies, standards, and procedures related to the security of the system are identified;
+[c] managers, systems administrators, and users of the system are made aware of the security risks associated with their activities; and
+[d] managers, systems administrators, and users of the system are made aware of the applicable policies, standards, and procedures related to the security of the system.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] information security-related duties, roles, and responsibilities are defined;
+[b] information security-related duties, roles, and responsibilities are assigned to designated personnel; and
+[c] personnel are adequately trained to carry out their assigned information security-related duties, roles, and responsibilities.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] potential indicators associated with insider threats are identified; and
+[b] security awareness training on recognizing and reporting potential indicators of insider threat is provided to managers and employees.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] audit logs needed (i.e., event types to be logged) to enable the monitoring, analysis, investigation, and reporting of unlawful or unauthorized system activity are specified;
+[b] the content of audit records needed to support monitoring, analysis, investigation, and reporting of unlawful or unauthorized system activity is defined;
+[c] audit records are created (generated);
+[d] audit records, once created, contain the defined content;
+[e] retention requirements for audit records are defined; and
+[f] audit records are retained as defined.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the content of the audit records needed to support the ability to uniquely trace users to their actions is defined; and
+[b] audit records, once created, contain the defined content.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a process for determining when to review logged events is defined;
+[b] event types being logged are reviewed in accordance with the defined review process; and
+[c] event types being logged are updated based on the review.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] personnel or roles to be alerted in the event of an audit logging process failure are identified;
+[b] types of audit logging process failures for which alert will be generated are defined; and
+[c] identified personnel or roles are alerted in the event of an audit logging process failure.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] audit record review, analysis, and reporting processes for investigation and response to indications of unlawful, unauthorized, suspicious, or unusual activity are defined; and
+[b] defined audit record review, analysis, and reporting processes are correlated.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] an audit record reduction capability that supports on-demand analysis is provided; and
+[b] a report generation capability that supports on-demand reporting is provided.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] internal system clocks are used to generate time stamps for audit records;
+[b] an authoritative source with which to compare and synchronize internal system clocks is specified; and
+[c] internal system clocks used to generate time stamps for audit records are compared to and synchronized with the specified authoritative time source.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] audit information is protected from unauthorized access;
+[b] audit information is protected from unauthorized modification;
+[c] audit information is protected from unauthorized deletion;
+[d] audit logging tools are protected from unauthorized access;
+[e] audit logging tools are protected from unauthorized modification; and
+[f] audit logging tools are protected from unauthorized deletion.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a subset of privileged users granted access to manage audit logging functionality is defined; and
+[b] management of audit logging functionality is limited to the defined subset of privileged users.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a baseline configuration is established;
+[b] the baseline configuration includes hardware, software, firmware, and documentation;
+[c] the baseline configuration is maintained (reviewed and updated) throughout the system development life cycle;
+[d] a system inventory is established;
+[e] the system inventory includes hardware, software, firmware, and documentation; and
+[f] the inventory is maintained (reviewed and updated) throughout the system development life cycle.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] security configuration settings for information technology products employed in the system are established and included in the baseline configuration; and
+[b] security configuration settings for information technology products employed in the system are enforced.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] changes to the system are tracked;
+[b] changes to the system are reviewed;
+[c] changes to the system are approved or disapproved; and
+[d] changes to the system are logged.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the security impact of changes to the system is analyzed prior to implementation.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] physical access restrictions associated with changes to the system are defined;
+[b] physical access restrictions associated with changes to the system are documented;
+[c] physical access restrictions associated with changes to the system are approved;
+[d] physical access restrictions associated with changes to the system are enforced;
+[e] logical access restrictions associated with changes to the system are defined;
+[f] logical access restrictions associated with changes to the system are documented;
+[g] logical access restrictions associated with changes to the system are approved; and
+[h] logical access restrictions associated with changes to the system are enforced.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] essential system capabilities are defined based on the principle of least functionality; and
+[b] the system is configured to provide only the defined essential capabilities.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] essential programs are defined;
+[b] the use of nonessential programs is defined;
+[c] the use of nonessential programs is restricted, disabled, or prevented as defined;
+[d] essential functions are defined;
+[e] the use of nonessential functions is defined;
+[f] the use of nonessential functions is restricted, disabled, or prevented as defined;
+[g] essential ports are defined;
+[h] the use of nonessential ports is defined;
+[i] the use of nonessential ports is restricted, disabled, or prevented as defined;
+[j] essential protocols are defined;
+[k] the use of nonessential protocols is defined;
+[l] the use of nonessential protocols is restricted, disabled, or prevented as defined;
+[m] essential services are defined;
+[n] the use of nonessential services is defined; and
+[o] the use of nonessential services is restricted, disabled, or prevented as defined.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a policy specifying whether whitelisting or blacklisting is to be implemented is specified;
+[b] the software allowed to execute under whitelisting or denied use under blacklisting is specified; and
+[c] whitelisting to allow the execution of authorized software or blacklisting to prevent the use of unauthorized software is implemented as specified.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a policy for controlling the installation of software by users is established;
+[b] installation of software by users is controlled based on the established policy; and
+[c] installation of software by users is monitored.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] privileged accounts are identified;
+[b] multifactor authentication is implemented for local access to privileged accounts;
+[c] multifactor authentication is implemented for network access to privileged accounts; and
+[d] multifactor authentication is implemented for network access to non-privileged accounts.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] replay-resistant authentication mechanisms are implemented for network account access to privileged and non-privileged accounts.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a period within which identifiers cannot be reused is defined; and
+[b] reuse of identifiers is prevented within the defined period.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a period of inactivity after which an identifier is disabled is defined; and
+[b] identifiers are disabled after the defined period of inactivity.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] password complexity requirements are defined;
+[b] password change of character requirements are defined;
+[c] minimum password complexity requirements as defined are enforced when new passwords are created; and
+[d] minimum password change of character requirements as defined are enforced when new passwords are created.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the number of generations during which a password cannot be reused is specified and
+[b] reuse of passwords is prohibited during the specified number of generations.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] an immediate change to a permanent password is required when a temporary password is used for system logon.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] passwords are cryptographically protected in storage; and
+[b] passwords are cryptographically protected in transit.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] authentication information is obscured during the authentication process.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] an operational incident-handling capability is established;
+[b] the operational incident-handling capability includes preparation;
+[c] the operational incident-handling capability includes detection;
+[d] the operational incident-handling capability includes analysis;
+[e] the operational incident-handling capability includes containment;
+[f] the operational incident-handling capability includes recovery; and
+[g] the operational incident-handling capability includes user response activities.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] incidents are tracked;
+[b] incidents are documented;
+[c] authorities to whom incidents are to be reported are identified;
+[d] organizational officials to whom incidents are to be reported are identified;
+[e] identified authorities are notified of incidents; and
+[f] identified organizational officials are notified of incidents.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the incident response capability is tested.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] system maintenance is performed.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] tools used to conduct system maintenance are controlled;
+[b] techniques used to conduct system maintenance are controlled;
+[c] mechanisms used to conduct system maintenance are controlled; and
+[d] personnel used to conduct system maintenance are controlled.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] equipment to be removed from organizational spaces for off-site maintenance is sanitized of any CUI.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] media containing diagnostic and test programs are checked for malicious code before being used in organizational systems that process, store, or transmit CUI.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] multifactor authentication is used to establish nonlocal maintenance sessions via external network connections; and
+[b] nonlocal maintenance sessions established via external network connections are terminated when nonlocal maintenance is complete.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] maintenance personnel without required access authorization are supervised during maintenance activities.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] paper media containing CUI is physically controlled;
+[b] digital media containing CUI is physically controlled;
+[c] paper media containing CUI is securely stored; and
+[d] digital media containing CUI is securely stored.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] access to CUI on system media is limited to authorized users.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] media containing CUI is marked with applicable CUI markings; and
+[b] media containing CUI is marked with distribution limitations.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] access to media containing CUI is controlled; and
+[b] accountability for media containing CUI is maintained during transport outside of controlled areas.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the confidentiality of CUI stored on digital media is protected during transport using cryptographic mechanisms or alternative physical safeguards.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the use of removable media on system components is controlled.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the use of portable storage devices is prohibited when such devices have no identifiable owner.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the confidentiality of backup CUI is protected at storage locations.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] individuals are screened prior to authorizing access to organizational systems containing CUI.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a policy and/or process for terminating system access and any credentials coincident with personnel actions is established;
+[b] system access and credentials are terminated consistent with personnel actions such as termination or transfer; and
+[c] the system is protected during and after personnel transfer actions.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the physical facility where organizational systems reside is protected;
+[b] the support infrastructure for organizational systems is protected;
+[c] the physical facility where organizational systems reside is monitored; and
+[d] the support infrastructure for organizational systems is monitored.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] safeguarding measures for CUI are defined for alternate work sites; and
+[b] safeguarding measures for CUI are enforced for alternate work sites.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the frequency to assess risk to organizational operations, organizational assets, and individuals is defined; and
+[b] risk to organizational operations, organizational assets, and individuals resulting from the operation of an organizational system that processes, stores, or transmits CUI is assessed with the defined frequency.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the frequency to scan for vulnerabilities in organizational systems and applications is defined;
+[b] vulnerability scans are performed on organizational systems with the defined frequency;
+[c] vulnerability scans are performed on applications with the defined frequency;
+[d] vulnerability scans are performed on organizational systems when new vulnerabilities are identified; and
+[e] vulnerability scans are performed on applications when new vulnerabilities are identified.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] vulnerabilities are identified; and
+[b] vulnerabilities are remediated in accordance with risk assessments.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the frequency of security control assessments is defined; and
+[b] security controls are assessed with the defined frequency to determine if the controls are effective in their application.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] deficiencies and vulnerabilities to be addressed by the plan of action are identified;
+[b] a plan of action is developed to correct identified deficiencies and reduce or eliminate identified vulnerabilities; and
+[c] the plan of action is implemented to correct identified deficiencies and reduce or eliminate identified vulnerabilities.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] security controls are monitored on an ongoing basis to ensure the continued effectiveness of those controls.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a system security plan is developed;
+[b] the system boundary is described and documented in the system security plan;
+[c] the system environment of operation is described and documented in the system security plan;
+[d] the security requirements identified and approved by the designated authority as non-applicable are identified;
+[e] the method of security requirement implementation is described and documented in the system security plan;
+[f] the relationship with or connection to other systems is described and documented in the system security plan;
+[g] the frequency to update the system security plan is defined; and
+[h] system security plan is updated with the defined frequency.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] architectural designs that promote effective information security are identified;
+[b] software development techniques that promote effective information security are identified;
+[c] systems engineering principles that promote effective information security are identified;
+[d] identified architectural designs that promote effective information security are employed;
+[e] identified software development techniques that promote effective information security are employed; and
+[f] identified systems engineering principles that promote effective information security are employed.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] user functionality is identified;
+[b] system management functionality is identified; and
+[c] user functionality is separated from system management functionality.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] unauthorized and unintended information transfer via shared system resources is prevented.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] network communications traffic is denied by default; and
+[b] network communications traffic is allowed by exception.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] remote devices are prevented from simultaneously establishing non-remote connections with the system and communicating via some other connection to resources in external networks (i.e., split tunneling).</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] cryptographic mechanisms intended to prevent unauthorized disclosure of CUI are identified;
+[b] alternative physical safeguards intended to prevent unauthorized disclosure of CUI are identified; and
+[c] either cryptographic mechanisms or alternative physical safeguards are implemented to prevent unauthorized disclosure of CUI during transmission.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] a period of inactivity to terminate network connections associated with communications sessions is defined;
+[b] network connections associated with communications sessions are terminated at the end of the sessions; and
+[c] network connections associated with communications sessions are terminated after the defined period of inactivity.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] cryptographic keys are established whenever cryptography is employed; and
+[b] cryptographic keys are managed whenever cryptography is employed.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] FIPS-validated cryptography is employed to protect the confidentiality of CUI.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] collaborative computing devices are identified;
+[b] collaborative computing devices provide indication to users of devices in use; and
+[c] remote activation of collaborative computing devices is prohibited.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] use of mobile code is controlled; and
+[b] use of mobile code is monitored.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] use of Voice over Internet Protocol (VoIP) technologies is controlled; and
+[b] use of Voice over Internet Protocol (VoIP) technologies is monitored.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the authenticity of communications sessions is protected.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the confidentiality of CUI at rest is protected.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] response actions to system security alerts and advisories are identified;
+[b] system security alerts and advisories are monitored; and
+[c] actions in response to system security alerts and advisories are taken.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] the system is monitored to detect attacks and indicators of potential attacks;
+[b] inbound communications traffic is monitored to detect attacks and indicators of potential attacks; and
+[c] outbound communications traffic is monitored to detect attacks and indicators of potential attacks.</t>
+  </si>
+  <si>
+    <t>Determine if:
+[a] authorized use of the system is defined; and
+[b] unauthorized use of the system is identified.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1447,6 +2116,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1534,7 +2209,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1569,6 +2244,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1608,7 +2292,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -1904,10 +2588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D81E34-467D-454F-919D-D7D2498D893F}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="214" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1921,7 +2605,7 @@
         <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1929,7 +2613,7 @@
         <v>137</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1993,7 +2677,7 @@
         <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2045,6 +2729,17 @@
       </c>
       <c r="C16" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="C17" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -2054,10 +2749,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A200010B-5D7D-2948-822B-E40FF0ABA104}">
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G126" sqref="G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2065,11 +2760,13 @@
     <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="44.1640625" customWidth="1"/>
     <col min="5" max="5" width="133.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>165</v>
@@ -2083,11 +2780,14 @@
       <c r="E1" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6">
         <v>1</v>
       </c>
@@ -2098,447 +2798,513 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>397</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="238" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>398</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>398</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>398</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>398</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>398</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>398</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>398</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>398</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>398</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>398</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>398</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>398</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>398</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>398</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>398</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>398</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>398</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>397</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>398</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="6" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>397</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6">
         <v>1</v>
       </c>
@@ -2549,67 +3315,76 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>398</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>398</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>398</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="6">
         <v>1</v>
       </c>
@@ -2620,187 +3395,214 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="289" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>398</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>398</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D32" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>398</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>398</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>398</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D35" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>398</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D36" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>398</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>398</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>398</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6">
         <v>1</v>
       </c>
@@ -2810,191 +3612,215 @@
       <c r="D39" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F39" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:7" ht="289" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>398</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>398</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>398</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D43" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>398</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="388" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D44" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>398</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D45" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>398</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>398</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B47">
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D47" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>398</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B48">
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="6" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>398</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="6" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="6">
         <v>1</v>
       </c>
@@ -3005,227 +3831,260 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>397</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B51">
         <v>2</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>397</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>398</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>398</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B54">
         <v>2</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>398</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B55">
         <v>2</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>398</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B56">
         <v>2</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>398</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B57">
         <v>2</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>398</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B58">
         <v>2</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>398</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B59">
         <v>2</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>398</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B60">
         <v>2</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>398</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B61" s="6">
         <v>1</v>
       </c>
@@ -3236,67 +4095,76 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B62">
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D62" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>398</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B63">
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D63" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>398</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B64">
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D64" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>398</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="6">
         <v>1</v>
       </c>
@@ -3307,127 +4175,145 @@
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B66">
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D66" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>398</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B67">
         <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D67" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
+        <v>398</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B68">
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D68" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>398</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B69">
         <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D69" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>398</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B70">
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D70" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>398</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B71">
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D71" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F71" t="s">
+        <v>398</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B72" s="6">
         <v>1</v>
       </c>
@@ -3438,187 +4324,214 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B73">
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D73" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F73" t="s">
+        <v>398</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B74">
         <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D74" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F74" t="s">
+        <v>398</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B75">
         <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D75" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F75" t="s">
+        <v>397</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B76">
         <v>2</v>
       </c>
       <c r="C76" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D76" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>398</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B77">
         <v>2</v>
       </c>
       <c r="C77" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D77" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F77" t="s">
+        <v>398</v>
+      </c>
+      <c r="G77" s="12" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B78">
         <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D78" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F78">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F78" t="s">
+        <v>398</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B79">
         <v>2</v>
       </c>
       <c r="C79" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D79" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F79" t="s">
+        <v>398</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B80">
         <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D80" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F80">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F80" t="s">
+        <v>398</v>
+      </c>
+      <c r="G80" s="12" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B81">
         <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D81" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F81" t="s">
+        <v>398</v>
+      </c>
+      <c r="G81" s="12" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="6">
         <v>1</v>
       </c>
@@ -3629,47 +4542,53 @@
         <v>92</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B83">
         <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D83" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F83">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F83" t="s">
+        <v>398</v>
+      </c>
+      <c r="G83" s="12" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B84">
         <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D84" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F84" t="s">
+        <v>398</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B85" s="6">
         <v>1</v>
       </c>
@@ -3680,127 +4599,145 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B86">
         <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D86" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F86" t="s">
+        <v>397</v>
+      </c>
+      <c r="G86" s="12" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B87">
         <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D87" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F87">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F87" t="s">
+        <v>398</v>
+      </c>
+      <c r="G87" s="12" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B88">
         <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D88" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F88" t="s">
+        <v>397</v>
+      </c>
+      <c r="G88" s="12" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B89">
         <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D89" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F89" t="s">
+        <v>397</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B90">
         <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D90" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F90" t="s">
+        <v>397</v>
+      </c>
+      <c r="G90" s="12" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B91">
         <v>2</v>
       </c>
       <c r="C91" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D91" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F91" t="s">
+        <v>398</v>
+      </c>
+      <c r="G91" s="12" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B92" s="6">
         <v>1</v>
       </c>
@@ -3811,67 +4748,76 @@
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B93">
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D93" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F93">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F93" t="s">
+        <v>398</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B94">
         <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D94" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F94">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F94" t="s">
+        <v>398</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B95">
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D95" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F95">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F95" t="s">
+        <v>398</v>
+      </c>
+      <c r="G95" s="12" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B96" s="6">
         <v>1</v>
       </c>
@@ -3882,87 +4828,99 @@
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B97">
         <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D97" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F97">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F97" t="s">
+        <v>398</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B98">
         <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D98" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E98" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F98">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F98" t="s">
+        <v>398</v>
+      </c>
+      <c r="G98" s="12" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B99">
         <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D99" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E99" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F99">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F99" t="s">
+        <v>398</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="340" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B100">
         <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D100" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E100" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F100">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F100" t="s">
+        <v>398</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B101" s="6">
         <v>1</v>
       </c>
@@ -3973,327 +4931,375 @@
         <v>111</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="289" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B102">
         <v>2</v>
       </c>
       <c r="C102" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D102" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F102" t="s">
+        <v>397</v>
+      </c>
+      <c r="G102" s="12" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="306" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B103">
         <v>2</v>
       </c>
       <c r="C103" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D103" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F103">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F103" t="s">
+        <v>398</v>
+      </c>
+      <c r="G103" s="12" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B104">
         <v>2</v>
       </c>
       <c r="C104" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D104" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F104">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F104" t="s">
+        <v>398</v>
+      </c>
+      <c r="G104" s="12" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B105">
         <v>2</v>
       </c>
       <c r="C105" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D105" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F105">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F105" t="s">
+        <v>398</v>
+      </c>
+      <c r="G105" s="12" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B106">
         <v>2</v>
       </c>
       <c r="C106" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D106" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F106" t="s">
+        <v>397</v>
+      </c>
+      <c r="G106" s="12" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B107">
         <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D107" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F107">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F107" t="s">
+        <v>398</v>
+      </c>
+      <c r="G107" s="12" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B108">
         <v>2</v>
       </c>
       <c r="C108" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D108" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F108">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F108" t="s">
+        <v>398</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B109">
         <v>2</v>
       </c>
       <c r="C109" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D109" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F109">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F109" t="s">
+        <v>398</v>
+      </c>
+      <c r="G109" s="12" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B110">
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D110" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F110">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F110" t="s">
+        <v>398</v>
+      </c>
+      <c r="G110" s="12" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B111">
         <v>2</v>
       </c>
       <c r="C111" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D111" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F111">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F111" t="s">
+        <v>398</v>
+      </c>
+      <c r="G111" s="12" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B112">
         <v>2</v>
       </c>
       <c r="C112" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D112" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F112">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F112" t="s">
+        <v>398</v>
+      </c>
+      <c r="G112" s="12" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B113">
         <v>2</v>
       </c>
       <c r="C113" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D113" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F113">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F113" t="s">
+        <v>398</v>
+      </c>
+      <c r="G113" s="12" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B114">
         <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D114" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F114">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F114" t="s">
+        <v>398</v>
+      </c>
+      <c r="G114" s="12" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B115">
         <v>2</v>
       </c>
       <c r="C115" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D115" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F115">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F115" t="s">
+        <v>398</v>
+      </c>
+      <c r="G115" s="12" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B116">
         <v>2</v>
       </c>
       <c r="C116" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D116" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F116">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F116" t="s">
+        <v>398</v>
+      </c>
+      <c r="G116" s="12" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B117">
         <v>2</v>
       </c>
       <c r="C117" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D117" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F117">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F117" t="s">
+        <v>398</v>
+      </c>
+      <c r="G117" s="12" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B118" s="6">
         <v>1</v>
       </c>
@@ -4304,149 +5310,212 @@
         <v>128</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B119">
         <v>2</v>
       </c>
       <c r="C119" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D119" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F119" t="s">
+        <v>397</v>
+      </c>
+      <c r="G119" s="12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B120">
         <v>2</v>
       </c>
       <c r="C120" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D120" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F120" t="s">
+        <v>397</v>
+      </c>
+      <c r="G120" s="12" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B121">
         <v>2</v>
       </c>
       <c r="C121" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D121" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F121">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F121" t="s">
+        <v>398</v>
+      </c>
+      <c r="G121" s="12" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B122">
         <v>2</v>
       </c>
       <c r="C122" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D122" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="F122" t="s">
+        <v>397</v>
+      </c>
+      <c r="G122" s="12" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B123">
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D123" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F123" t="s">
+        <v>397</v>
+      </c>
+      <c r="G123" s="12" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B124">
         <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D124" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F124">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F124" t="s">
+        <v>398</v>
+      </c>
+      <c r="G124" s="12" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B125">
         <v>2</v>
       </c>
       <c r="C125" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D125" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F125">
-        <v>2</v>
+      <c r="F125" t="s">
+        <v>398</v>
+      </c>
+      <c r="G125" s="12" t="s">
+        <v>509</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE94727-C240-9D4C-A77B-C9C25836C1E1}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4460,6 +5529,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <EmailTo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailHeaders xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <EmailSender xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailFrom xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailSubject xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailCc xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002B3F23EB2048A24987DC8CE7E89BA2CA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="57ee07fa861f4d000c01c5387baf5e7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="8d3f00d4-6cb9-4a73-b6cd-69039b4132b3" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a39b6d99b357596f1f139bb8b3efd27" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4659,19 +5741,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <EmailTo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailHeaders xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <EmailSender xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailFrom xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailSubject xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailCc xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{594FD6D8-8812-4CA3-A4C2-A9F4F741D298}">
   <ds:schemaRefs>
@@ -4681,6 +5750,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A49C780-D6EE-4F9B-A1B2-2AF8E74E99DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8d3f00d4-6cb9-4a73-b6cd-69039b4132b3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AD64251-3E42-4101-9445-91DF49E57B98}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4698,22 +5785,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A49C780-D6EE-4F9B-A1B2-2AF8E74E99DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8d3f00d4-6cb9-4a73-b6cd-69039b4132b3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>